<commit_message>
Criação da tela de Categoria
</commit_message>
<xml_diff>
--- a/Auxiliar/Dicionario MiniProjeto.xlsx
+++ b/Auxiliar/Dicionario MiniProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johann.bdticona\source\repos\C#\Noite\MiniProjeto\MiniProjeto\Auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEC4BA3-D99B-480C-A903-D308CB890E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1AB5E1-98F0-481A-8E5F-50E8B186497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{0C592CAE-E485-4091-B840-E6915182917B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="69">
   <si>
     <t>tabela</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>txtCodigo</t>
+  </si>
+  <si>
+    <t>txtDescricao</t>
   </si>
 </sst>
 </file>
@@ -2008,7 +2011,7 @@
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,7 +2096,7 @@
         <v>61</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" ref="Q4:S9" si="1">""""&amp;B4&amp;"_"&amp;$C$1&amp;","""&amp;" +"</f>
+        <f t="shared" ref="Q4:Q9" si="1">""""&amp;B4&amp;"_"&amp;$C$1&amp;","""&amp;" +"</f>
         <v>"nome_usuario," +</v>
       </c>
       <c r="S4" t="str">
@@ -2288,6 +2291,9 @@
         <f>B13&amp;"_"&amp;$C$11&amp;" "&amp;C13&amp;" "&amp;D13&amp;" "&amp;E13&amp;","</f>
         <v>id_categoria int not null identity primary key,</v>
       </c>
+      <c r="O13" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -2306,6 +2312,9 @@
         <f t="shared" ref="I14:I17" si="3">B14&amp;"_"&amp;$C$11&amp;" "&amp;C14&amp;" "&amp;D14&amp;" "&amp;E14&amp;","</f>
         <v>nome_categoria varchar(50) not null unique,</v>
       </c>
+      <c r="O14" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -2321,6 +2330,9 @@
         <f t="shared" si="3"/>
         <v>descricao_categoria varchar(255) not null ,</v>
       </c>
+      <c r="O15" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -2336,8 +2348,11 @@
         <f t="shared" si="3"/>
         <v>status_categoria varchar(30) not null ,</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -2351,8 +2366,11 @@
         <f t="shared" si="3"/>
         <v>obs_categoria varchar(255) null ,</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2363,7 +2381,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2383,7 +2401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2404,7 +2422,7 @@
         <v>id_produto int not null identity primary key,</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -2422,7 +2440,7 @@
         <v>id_categoria_produto int not null ,</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -2440,7 +2458,7 @@
         <v>nome_produto varchar(50) not null unique,</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>30</v>
       </c>
@@ -2455,7 +2473,7 @@
         <v>qtde_produto int not null ,</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>31</v>
       </c>
@@ -2470,7 +2488,7 @@
         <v>peso_produto decimal(10,3) not null ,</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>32</v>
       </c>
@@ -2485,7 +2503,7 @@
         <v>unidade_produto varchar(30) not null ,</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>33</v>
       </c>
@@ -2503,7 +2521,7 @@
         <v>cadastro_produto smalldatetime not null default getdate(),</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>34</v>
       </c>
@@ -2518,7 +2536,7 @@
         <v>valorCusto_produto decimal(10,2) not null ,</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>35</v>
       </c>
@@ -2533,7 +2551,7 @@
         <v>valorVenda_produto decimal(10,2) not null ,</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>18</v>
       </c>
@@ -2548,7 +2566,7 @@
         <v>status_produto varchar(30) not null ,</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Codificação da tela de Categoria
</commit_message>
<xml_diff>
--- a/Auxiliar/Dicionario MiniProjeto.xlsx
+++ b/Auxiliar/Dicionario MiniProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johann.bdticona\source\repos\C#\Noite\MiniProjeto\MiniProjeto\Auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1AB5E1-98F0-481A-8E5F-50E8B186497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FE3AE4-0616-4515-8234-6A4A0A60CE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{0C592CAE-E485-4091-B840-E6915182917B}"/>
   </bookViews>
@@ -2011,7 +2011,7 @@
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="S13" sqref="S13:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,6 +2294,14 @@
       <c r="O13" t="s">
         <v>67</v>
       </c>
+      <c r="Q13" t="str">
+        <f>""""&amp;B13&amp;"_"&amp;$C$11&amp;","""&amp;" +"</f>
+        <v>"id_categoria," +</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" ref="S13:S18" si="3">"""'"""&amp;"+"&amp;O13&amp;".Text"&amp;"+""',"""&amp;"+"</f>
+        <v>"'"+txtCodigo.Text+"',"+</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -2309,11 +2317,19 @@
         <v>24</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" ref="I14:I17" si="3">B14&amp;"_"&amp;$C$11&amp;" "&amp;C14&amp;" "&amp;D14&amp;" "&amp;E14&amp;","</f>
+        <f t="shared" ref="I14:I17" si="4">B14&amp;"_"&amp;$C$11&amp;" "&amp;C14&amp;" "&amp;D14&amp;" "&amp;E14&amp;","</f>
         <v>nome_categoria varchar(50) not null unique,</v>
       </c>
       <c r="O14" t="s">
         <v>61</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" ref="Q14:Q17" si="5">""""&amp;B14&amp;"_"&amp;$C$11&amp;","""&amp;" +"</f>
+        <v>"nome_categoria," +</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="3"/>
+        <v>"'"+txtNome.Text+"',"+</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2327,11 +2343,19 @@
         <v>11</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>descricao_categoria varchar(255) not null ,</v>
       </c>
       <c r="O15" t="s">
         <v>68</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="5"/>
+        <v>"descricao_categoria," +</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="3"/>
+        <v>"'"+txtDescricao.Text+"',"+</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2345,14 +2369,22 @@
         <v>11</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>status_categoria varchar(30) not null ,</v>
       </c>
       <c r="O16" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16" t="str">
+        <f t="shared" si="5"/>
+        <v>"status_categoria," +</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" si="3"/>
+        <v>"'"+cboStatus.Text+"',"+</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -2363,14 +2395,22 @@
         <v>23</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>obs_categoria varchar(255) null ,</v>
       </c>
       <c r="O17" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17" t="str">
+        <f t="shared" si="5"/>
+        <v>"obs_categoria," +</v>
+      </c>
+      <c r="S17" t="str">
+        <f t="shared" si="3"/>
+        <v>"'"+txtObs.Text+"',"+</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2381,7 +2421,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2401,7 +2441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2422,7 +2462,7 @@
         <v>id_produto int not null identity primary key,</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -2436,11 +2476,11 @@
         <v>11</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" ref="I22:I31" si="4">B22&amp;"_"&amp;$C$19&amp;" "&amp;C22&amp;" "&amp;D22&amp;" "&amp;E22&amp;","</f>
+        <f t="shared" ref="I22:I31" si="6">B22&amp;"_"&amp;$C$19&amp;" "&amp;C22&amp;" "&amp;D22&amp;" "&amp;E22&amp;","</f>
         <v>id_categoria_produto int not null ,</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -2454,11 +2494,11 @@
         <v>24</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>nome_produto varchar(50) not null unique,</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>30</v>
       </c>
@@ -2469,11 +2509,11 @@
         <v>11</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>qtde_produto int not null ,</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>31</v>
       </c>
@@ -2484,11 +2524,11 @@
         <v>11</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>peso_produto decimal(10,3) not null ,</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>32</v>
       </c>
@@ -2499,11 +2539,11 @@
         <v>11</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>unidade_produto varchar(30) not null ,</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>33</v>
       </c>
@@ -2517,11 +2557,11 @@
         <v>37</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cadastro_produto smalldatetime not null default getdate(),</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>34</v>
       </c>
@@ -2532,11 +2572,11 @@
         <v>11</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>valorCusto_produto decimal(10,2) not null ,</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>35</v>
       </c>
@@ -2547,11 +2587,11 @@
         <v>11</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>valorVenda_produto decimal(10,2) not null ,</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>18</v>
       </c>
@@ -2562,11 +2602,11 @@
         <v>11</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>status_produto varchar(30) not null ,</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>17</v>
       </c>
@@ -2577,7 +2617,7 @@
         <v>23</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>obs_produto varchar(255) null ,</v>
       </c>
     </row>
@@ -2647,7 +2687,7 @@
         <v>11</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" ref="I36:I43" si="5">B36&amp;"_"&amp;$C$33&amp;" "&amp;C36&amp;" "&amp;D36&amp;" "&amp;E36&amp;","</f>
+        <f t="shared" ref="I36:I43" si="7">B36&amp;"_"&amp;$C$33&amp;" "&amp;C36&amp;" "&amp;D36&amp;" "&amp;E36&amp;","</f>
         <v>id_produto_movProduto int not null ,</v>
       </c>
     </row>
@@ -2665,7 +2705,7 @@
         <v>11</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>id_usuario_movProduto int not null ,</v>
       </c>
     </row>
@@ -2680,7 +2720,7 @@
         <v>11</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>qtde_movProduto int not null ,</v>
       </c>
     </row>
@@ -2698,7 +2738,7 @@
         <v>37</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>cadastro_movProduto smalldatetime not null default getdate(),</v>
       </c>
     </row>
@@ -2713,7 +2753,7 @@
         <v>11</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>tipo_movProduto varchar(30) not null ,</v>
       </c>
     </row>
@@ -2728,7 +2768,7 @@
         <v>11</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>descricao_movProduto varchar(255) not null ,</v>
       </c>
     </row>
@@ -2743,7 +2783,7 @@
         <v>11</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>status_movProduto varchar(30) not null ,</v>
       </c>
     </row>
@@ -2758,7 +2798,7 @@
         <v>23</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>obs_movProduto varchar(255) null ,</v>
       </c>
     </row>
@@ -2828,7 +2868,7 @@
         <v>24</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" ref="I48:I55" si="6">B48&amp;"_"&amp;$C$45&amp;" "&amp;C48&amp;" "&amp;D48&amp;" "&amp;E48&amp;","</f>
+        <f t="shared" ref="I48:I55" si="8">B48&amp;"_"&amp;$C$45&amp;" "&amp;C48&amp;" "&amp;D48&amp;" "&amp;E48&amp;","</f>
         <v>cnpj_fornecedor char(18) not null unique,</v>
       </c>
     </row>
@@ -2843,7 +2883,7 @@
         <v>11</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>nome_fornecedor varchar(50) not null ,</v>
       </c>
     </row>
@@ -2858,7 +2898,7 @@
         <v>11</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cep_fornecedor char(9) not null ,</v>
       </c>
     </row>
@@ -2873,7 +2913,7 @@
         <v>11</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>numero_fornecedor int not null ,</v>
       </c>
     </row>
@@ -2888,7 +2928,7 @@
         <v>11</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>telefone1_fornecedor char(14) not null ,</v>
       </c>
     </row>
@@ -2903,7 +2943,7 @@
         <v>11</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>telefone2_fornecedor char(14) not null ,</v>
       </c>
     </row>
@@ -2918,7 +2958,7 @@
         <v>11</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>status_fornecedor varchar(30) not null ,</v>
       </c>
     </row>
@@ -2933,7 +2973,7 @@
         <v>23</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>obs_fornecedor varchar(255) null ,</v>
       </c>
     </row>
@@ -3003,7 +3043,7 @@
         <v>11</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" ref="I60:I65" si="7">B60&amp;"_"&amp;$C$57&amp;" "&amp;C60&amp;" "&amp;D60&amp;" "&amp;E60&amp;","</f>
+        <f t="shared" ref="I60:I65" si="9">B60&amp;"_"&amp;$C$57&amp;" "&amp;C60&amp;" "&amp;D60&amp;" "&amp;E60&amp;","</f>
         <v>id_fornecedor_prodFornecedor int not null ,</v>
       </c>
     </row>
@@ -3021,7 +3061,7 @@
         <v>11</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>id_produto_prodFornecedor int not null ,</v>
       </c>
     </row>
@@ -3039,7 +3079,7 @@
         <v>37</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>dataEntrada_prodFornecedor smalldatetime not null default getdate(),</v>
       </c>
     </row>
@@ -3054,7 +3094,7 @@
         <v>11</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>descricao_prodFornecedor varchar(255) not null ,</v>
       </c>
     </row>
@@ -3069,7 +3109,7 @@
         <v>11</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>status_prodFornecedor varchar(30) not null ,</v>
       </c>
     </row>
@@ -3084,7 +3124,7 @@
         <v>23</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>obs_prodFornecedor varchar(255) null ,</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Criação da tela de Produto
</commit_message>
<xml_diff>
--- a/Auxiliar/Dicionario MiniProjeto.xlsx
+++ b/Auxiliar/Dicionario MiniProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johann.bdticona\source\repos\C#\Noite\MiniProjeto\MiniProjeto\Auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FE3AE4-0616-4515-8234-6A4A0A60CE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C963FE-AD74-4FC1-B160-10C8455C4B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{0C592CAE-E485-4091-B840-E6915182917B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="76">
   <si>
     <t>tabela</t>
   </si>
@@ -244,6 +244,27 @@
   </si>
   <si>
     <t>txtDescricao</t>
+  </si>
+  <si>
+    <t>txtCodigoCategoria</t>
+  </si>
+  <si>
+    <t>txtQtde</t>
+  </si>
+  <si>
+    <t>txtPeso</t>
+  </si>
+  <si>
+    <t>txtUnidade</t>
+  </si>
+  <si>
+    <t>txtCadastro</t>
+  </si>
+  <si>
+    <t>txtCusto</t>
+  </si>
+  <si>
+    <t>txtVenda</t>
   </si>
 </sst>
 </file>
@@ -2010,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B5DEC8-BB98-4C5A-8EDE-BF51A128181C}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13:S17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2299,7 +2320,7 @@
         <v>"id_categoria," +</v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" ref="S13:S18" si="3">"""'"""&amp;"+"&amp;O13&amp;".Text"&amp;"+""',"""&amp;"+"</f>
+        <f t="shared" ref="S13:S17" si="3">"""'"""&amp;"+"&amp;O13&amp;".Text"&amp;"+""',"""&amp;"+"</f>
         <v>"'"+txtCodigo.Text+"',"+</v>
       </c>
     </row>
@@ -2461,6 +2482,13 @@
         <f>B21&amp;"_"&amp;$C$19&amp;" "&amp;C21&amp;" "&amp;D21&amp;" "&amp;E21&amp;","</f>
         <v>id_produto int not null identity primary key,</v>
       </c>
+      <c r="O21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q21" t="str">
+        <f>""""&amp;B21&amp;"_"&amp;$C$19&amp;","""&amp;" +"</f>
+        <v>"id_produto," +</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2479,6 +2507,13 @@
         <f t="shared" ref="I22:I31" si="6">B22&amp;"_"&amp;$C$19&amp;" "&amp;C22&amp;" "&amp;D22&amp;" "&amp;E22&amp;","</f>
         <v>id_categoria_produto int not null ,</v>
       </c>
+      <c r="O22" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" ref="Q22:Q31" si="7">""""&amp;B22&amp;"_"&amp;$C$19&amp;","""&amp;" +"</f>
+        <v>"id_categoria_produto," +</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -2497,6 +2532,13 @@
         <f t="shared" si="6"/>
         <v>nome_produto varchar(50) not null unique,</v>
       </c>
+      <c r="O23" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="7"/>
+        <v>"nome_produto," +</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2512,6 +2554,13 @@
         <f t="shared" si="6"/>
         <v>qtde_produto int not null ,</v>
       </c>
+      <c r="O24" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="7"/>
+        <v>"qtde_produto," +</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -2527,6 +2576,13 @@
         <f t="shared" si="6"/>
         <v>peso_produto decimal(10,3) not null ,</v>
       </c>
+      <c r="O25" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="7"/>
+        <v>"peso_produto," +</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -2542,6 +2598,13 @@
         <f t="shared" si="6"/>
         <v>unidade_produto varchar(30) not null ,</v>
       </c>
+      <c r="O26" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="7"/>
+        <v>"unidade_produto," +</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -2560,6 +2623,13 @@
         <f t="shared" si="6"/>
         <v>cadastro_produto smalldatetime not null default getdate(),</v>
       </c>
+      <c r="O27" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="7"/>
+        <v>"cadastro_produto," +</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -2575,6 +2645,13 @@
         <f t="shared" si="6"/>
         <v>valorCusto_produto decimal(10,2) not null ,</v>
       </c>
+      <c r="O28" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="7"/>
+        <v>"valorCusto_produto," +</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -2590,6 +2667,13 @@
         <f t="shared" si="6"/>
         <v>valorVenda_produto decimal(10,2) not null ,</v>
       </c>
+      <c r="O29" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="7"/>
+        <v>"valorVenda_produto," +</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -2605,6 +2689,13 @@
         <f t="shared" si="6"/>
         <v>status_produto varchar(30) not null ,</v>
       </c>
+      <c r="O30" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="7"/>
+        <v>"status_produto," +</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -2620,6 +2711,13 @@
         <f t="shared" si="6"/>
         <v>obs_produto varchar(255) null ,</v>
       </c>
+      <c r="O31" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="7"/>
+        <v>"obs_produto," +</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -2687,7 +2785,7 @@
         <v>11</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" ref="I36:I43" si="7">B36&amp;"_"&amp;$C$33&amp;" "&amp;C36&amp;" "&amp;D36&amp;" "&amp;E36&amp;","</f>
+        <f t="shared" ref="I36:I43" si="8">B36&amp;"_"&amp;$C$33&amp;" "&amp;C36&amp;" "&amp;D36&amp;" "&amp;E36&amp;","</f>
         <v>id_produto_movProduto int not null ,</v>
       </c>
     </row>
@@ -2705,7 +2803,7 @@
         <v>11</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>id_usuario_movProduto int not null ,</v>
       </c>
     </row>
@@ -2720,7 +2818,7 @@
         <v>11</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>qtde_movProduto int not null ,</v>
       </c>
     </row>
@@ -2738,7 +2836,7 @@
         <v>37</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cadastro_movProduto smalldatetime not null default getdate(),</v>
       </c>
     </row>
@@ -2753,7 +2851,7 @@
         <v>11</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>tipo_movProduto varchar(30) not null ,</v>
       </c>
     </row>
@@ -2768,7 +2866,7 @@
         <v>11</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>descricao_movProduto varchar(255) not null ,</v>
       </c>
     </row>
@@ -2783,7 +2881,7 @@
         <v>11</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>status_movProduto varchar(30) not null ,</v>
       </c>
     </row>
@@ -2798,7 +2896,7 @@
         <v>23</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>obs_movProduto varchar(255) null ,</v>
       </c>
     </row>
@@ -2868,7 +2966,7 @@
         <v>24</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" ref="I48:I55" si="8">B48&amp;"_"&amp;$C$45&amp;" "&amp;C48&amp;" "&amp;D48&amp;" "&amp;E48&amp;","</f>
+        <f t="shared" ref="I48:I55" si="9">B48&amp;"_"&amp;$C$45&amp;" "&amp;C48&amp;" "&amp;D48&amp;" "&amp;E48&amp;","</f>
         <v>cnpj_fornecedor char(18) not null unique,</v>
       </c>
     </row>
@@ -2883,7 +2981,7 @@
         <v>11</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>nome_fornecedor varchar(50) not null ,</v>
       </c>
     </row>
@@ -2898,7 +2996,7 @@
         <v>11</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>cep_fornecedor char(9) not null ,</v>
       </c>
     </row>
@@ -2913,7 +3011,7 @@
         <v>11</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>numero_fornecedor int not null ,</v>
       </c>
     </row>
@@ -2928,7 +3026,7 @@
         <v>11</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>telefone1_fornecedor char(14) not null ,</v>
       </c>
     </row>
@@ -2943,7 +3041,7 @@
         <v>11</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>telefone2_fornecedor char(14) not null ,</v>
       </c>
     </row>
@@ -2958,7 +3056,7 @@
         <v>11</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>status_fornecedor varchar(30) not null ,</v>
       </c>
     </row>
@@ -2973,7 +3071,7 @@
         <v>23</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>obs_fornecedor varchar(255) null ,</v>
       </c>
     </row>
@@ -3043,7 +3141,7 @@
         <v>11</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" ref="I60:I65" si="9">B60&amp;"_"&amp;$C$57&amp;" "&amp;C60&amp;" "&amp;D60&amp;" "&amp;E60&amp;","</f>
+        <f t="shared" ref="I60:I65" si="10">B60&amp;"_"&amp;$C$57&amp;" "&amp;C60&amp;" "&amp;D60&amp;" "&amp;E60&amp;","</f>
         <v>id_fornecedor_prodFornecedor int not null ,</v>
       </c>
     </row>
@@ -3061,7 +3159,7 @@
         <v>11</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>id_produto_prodFornecedor int not null ,</v>
       </c>
     </row>
@@ -3079,7 +3177,7 @@
         <v>37</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>dataEntrada_prodFornecedor smalldatetime not null default getdate(),</v>
       </c>
     </row>
@@ -3094,7 +3192,7 @@
         <v>11</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>descricao_prodFornecedor varchar(255) not null ,</v>
       </c>
     </row>
@@ -3109,7 +3207,7 @@
         <v>11</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>status_prodFornecedor varchar(30) not null ,</v>
       </c>
     </row>
@@ -3124,7 +3222,7 @@
         <v>23</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>obs_prodFornecedor varchar(255) null ,</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Codificação do botão Cadastro na tela Produto
</commit_message>
<xml_diff>
--- a/Auxiliar/Dicionario MiniProjeto.xlsx
+++ b/Auxiliar/Dicionario MiniProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johann.bdticona\source\repos\C#\Noite\MiniProjeto\MiniProjeto\Auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C963FE-AD74-4FC1-B160-10C8455C4B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA70650-D3A4-44AB-BA2F-1BA9FBE36E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{0C592CAE-E485-4091-B840-E6915182917B}"/>
   </bookViews>
@@ -249,9 +249,6 @@
     <t>txtCodigoCategoria</t>
   </si>
   <si>
-    <t>txtQtde</t>
-  </si>
-  <si>
     <t>txtPeso</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>txtVenda</t>
+  </si>
+  <si>
+    <t>numQtde</t>
   </si>
 </sst>
 </file>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B5DEC8-BB98-4C5A-8EDE-BF51A128181C}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,6 +2489,10 @@
         <f>""""&amp;B21&amp;"_"&amp;$C$19&amp;","""&amp;" +"</f>
         <v>"id_produto," +</v>
       </c>
+      <c r="S21" t="str">
+        <f>"""'"""&amp;"+"&amp;O21&amp;".Text"&amp;"+""',"""&amp;"+"</f>
+        <v>"'"+txtCodigo.Text+"',"+</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2514,6 +2518,10 @@
         <f t="shared" ref="Q22:Q31" si="7">""""&amp;B22&amp;"_"&amp;$C$19&amp;","""&amp;" +"</f>
         <v>"id_categoria_produto," +</v>
       </c>
+      <c r="S22" t="str">
+        <f t="shared" ref="S22:S31" si="8">"""'"""&amp;"+"&amp;O22&amp;".Text"&amp;"+""',"""&amp;"+"</f>
+        <v>"'"+txtCodigoCategoria.Text+"',"+</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -2539,6 +2547,10 @@
         <f t="shared" si="7"/>
         <v>"nome_produto," +</v>
       </c>
+      <c r="S23" t="str">
+        <f t="shared" si="8"/>
+        <v>"'"+txtNome.Text+"',"+</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2555,12 +2567,16 @@
         <v>qtde_produto int not null ,</v>
       </c>
       <c r="O24" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="7"/>
         <v>"qtde_produto," +</v>
       </c>
+      <c r="S24" t="str">
+        <f t="shared" si="8"/>
+        <v>"'"+numQtde.Text+"',"+</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -2577,12 +2593,16 @@
         <v>peso_produto decimal(10,3) not null ,</v>
       </c>
       <c r="O25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="7"/>
         <v>"peso_produto," +</v>
       </c>
+      <c r="S25" t="str">
+        <f t="shared" si="8"/>
+        <v>"'"+txtPeso.Text+"',"+</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -2599,12 +2619,16 @@
         <v>unidade_produto varchar(30) not null ,</v>
       </c>
       <c r="O26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="7"/>
         <v>"unidade_produto," +</v>
       </c>
+      <c r="S26" t="str">
+        <f t="shared" si="8"/>
+        <v>"'"+txtUnidade.Text+"',"+</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -2624,12 +2648,16 @@
         <v>cadastro_produto smalldatetime not null default getdate(),</v>
       </c>
       <c r="O27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="7"/>
         <v>"cadastro_produto," +</v>
       </c>
+      <c r="S27" t="str">
+        <f t="shared" si="8"/>
+        <v>"'"+txtCadastro.Text+"',"+</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -2646,12 +2674,16 @@
         <v>valorCusto_produto decimal(10,2) not null ,</v>
       </c>
       <c r="O28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="7"/>
         <v>"valorCusto_produto," +</v>
       </c>
+      <c r="S28" t="str">
+        <f t="shared" si="8"/>
+        <v>"'"+txtCusto.Text+"',"+</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -2668,12 +2700,16 @@
         <v>valorVenda_produto decimal(10,2) not null ,</v>
       </c>
       <c r="O29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q29" t="str">
         <f t="shared" si="7"/>
         <v>"valorVenda_produto," +</v>
       </c>
+      <c r="S29" t="str">
+        <f t="shared" si="8"/>
+        <v>"'"+txtVenda.Text+"',"+</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -2696,6 +2732,10 @@
         <f t="shared" si="7"/>
         <v>"status_produto," +</v>
       </c>
+      <c r="S30" t="str">
+        <f t="shared" si="8"/>
+        <v>"'"+cboStatus.Text+"',"+</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -2718,6 +2758,10 @@
         <f t="shared" si="7"/>
         <v>"obs_produto," +</v>
       </c>
+      <c r="S31" t="str">
+        <f t="shared" si="8"/>
+        <v>"'"+txtObs.Text+"',"+</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -2785,7 +2829,7 @@
         <v>11</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" ref="I36:I43" si="8">B36&amp;"_"&amp;$C$33&amp;" "&amp;C36&amp;" "&amp;D36&amp;" "&amp;E36&amp;","</f>
+        <f t="shared" ref="I36:I43" si="9">B36&amp;"_"&amp;$C$33&amp;" "&amp;C36&amp;" "&amp;D36&amp;" "&amp;E36&amp;","</f>
         <v>id_produto_movProduto int not null ,</v>
       </c>
     </row>
@@ -2803,7 +2847,7 @@
         <v>11</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>id_usuario_movProduto int not null ,</v>
       </c>
     </row>
@@ -2818,7 +2862,7 @@
         <v>11</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>qtde_movProduto int not null ,</v>
       </c>
     </row>
@@ -2836,7 +2880,7 @@
         <v>37</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>cadastro_movProduto smalldatetime not null default getdate(),</v>
       </c>
     </row>
@@ -2851,7 +2895,7 @@
         <v>11</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>tipo_movProduto varchar(30) not null ,</v>
       </c>
     </row>
@@ -2866,7 +2910,7 @@
         <v>11</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>descricao_movProduto varchar(255) not null ,</v>
       </c>
     </row>
@@ -2881,7 +2925,7 @@
         <v>11</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>status_movProduto varchar(30) not null ,</v>
       </c>
     </row>
@@ -2896,7 +2940,7 @@
         <v>23</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>obs_movProduto varchar(255) null ,</v>
       </c>
     </row>
@@ -2966,7 +3010,7 @@
         <v>24</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" ref="I48:I55" si="9">B48&amp;"_"&amp;$C$45&amp;" "&amp;C48&amp;" "&amp;D48&amp;" "&amp;E48&amp;","</f>
+        <f t="shared" ref="I48:I55" si="10">B48&amp;"_"&amp;$C$45&amp;" "&amp;C48&amp;" "&amp;D48&amp;" "&amp;E48&amp;","</f>
         <v>cnpj_fornecedor char(18) not null unique,</v>
       </c>
     </row>
@@ -2981,7 +3025,7 @@
         <v>11</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>nome_fornecedor varchar(50) not null ,</v>
       </c>
     </row>
@@ -2996,7 +3040,7 @@
         <v>11</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>cep_fornecedor char(9) not null ,</v>
       </c>
     </row>
@@ -3011,7 +3055,7 @@
         <v>11</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>numero_fornecedor int not null ,</v>
       </c>
     </row>
@@ -3026,7 +3070,7 @@
         <v>11</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>telefone1_fornecedor char(14) not null ,</v>
       </c>
     </row>
@@ -3041,7 +3085,7 @@
         <v>11</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>telefone2_fornecedor char(14) not null ,</v>
       </c>
     </row>
@@ -3056,7 +3100,7 @@
         <v>11</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>status_fornecedor varchar(30) not null ,</v>
       </c>
     </row>
@@ -3071,7 +3115,7 @@
         <v>23</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>obs_fornecedor varchar(255) null ,</v>
       </c>
     </row>
@@ -3141,7 +3185,7 @@
         <v>11</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" ref="I60:I65" si="10">B60&amp;"_"&amp;$C$57&amp;" "&amp;C60&amp;" "&amp;D60&amp;" "&amp;E60&amp;","</f>
+        <f t="shared" ref="I60:I65" si="11">B60&amp;"_"&amp;$C$57&amp;" "&amp;C60&amp;" "&amp;D60&amp;" "&amp;E60&amp;","</f>
         <v>id_fornecedor_prodFornecedor int not null ,</v>
       </c>
     </row>
@@ -3159,7 +3203,7 @@
         <v>11</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>id_produto_prodFornecedor int not null ,</v>
       </c>
     </row>
@@ -3177,7 +3221,7 @@
         <v>37</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>dataEntrada_prodFornecedor smalldatetime not null default getdate(),</v>
       </c>
     </row>
@@ -3192,7 +3236,7 @@
         <v>11</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>descricao_prodFornecedor varchar(255) not null ,</v>
       </c>
     </row>
@@ -3207,7 +3251,7 @@
         <v>11</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>status_prodFornecedor varchar(30) not null ,</v>
       </c>
     </row>
@@ -3222,7 +3266,7 @@
         <v>23</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>obs_prodFornecedor varchar(255) null ,</v>
       </c>
     </row>

</xml_diff>